<commit_message>
Added 5 TestCases with excel and csv.
</commit_message>
<xml_diff>
--- a/test_data/excel.xlsx
+++ b/test_data/excel.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\150286\Python BootCamp\hybrid_framework_web\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{365C0C0D-9F71-4B04-B2FD-5F4E8D495BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F86D83C-E83F-400E-B90F-E7FF914799D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4E01A38F-ABF4-483F-A6E5-A9956D75A07E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4E01A38F-ABF4-483F-A6E5-A9956D75A07E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>email</t>
   </si>
@@ -48,24 +49,28 @@
   </si>
   <si>
     <t>demo@123</t>
+  </si>
+  <si>
+    <t>null_shopping_cart</t>
+  </si>
+  <si>
+    <t>You have no items in your shopping cart.</t>
+  </si>
+  <si>
+    <t>book_name</t>
+  </si>
+  <si>
+    <t>Computing and Internet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -88,16 +93,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -410,32 +412,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D747ED4D-E4C2-4A57-8684-C2C02916C473}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -445,4 +455,57 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FE868F1-8858-4A2C-B2CE-E880BB9071A5}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{E900392B-24D7-4587-89D6-940BB1DDF3E9}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{4AFC9EC1-C34C-4EB1-AC7F-70C8726DE5BA}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>